<commit_message>
chore(listini): update Listino Simac.xlsx and CSV (Foglio1)
</commit_message>
<xml_diff>
--- a/preventivatore/mirror/data/Listino Simac.xlsx
+++ b/preventivatore/mirror/data/Listino Simac.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giuseppe/CascadeProjects/utenze-easy-page/preventivatore/mirror/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD18DCF-5E39-0D4D-82E7-EBEC79ECF275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5AA8FC-4244-DF49-9642-2CC5D1917F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="16640" xr2:uid="{49B5277E-39AE-3E49-A8BF-50ADC84C25A0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="70">
   <si>
     <t>Valore contratto</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>Potenza batteria</t>
+  </si>
+  <si>
+    <t>FTV 30 20 SGW</t>
+  </si>
+  <si>
+    <t>30 Kw</t>
   </si>
 </sst>
 </file>
@@ -644,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DBBB2D-4E20-B948-9566-E66BFB5B55C0}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -760,11 +766,11 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="4">
-        <f t="shared" ref="J3:J39" si="0">L3+K3</f>
+        <f t="shared" ref="J3:J40" si="0">L3+K3</f>
         <v>22299.22</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" ref="K3:K39" si="1">L3*0.06</f>
+        <f t="shared" ref="K3:K40" si="1">L3*0.06</f>
         <v>1262.22</v>
       </c>
       <c r="L3" s="4">
@@ -2069,11 +2075,48 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E40" s="2"/>
-      <c r="I40" s="2"/>
+      <c r="A40" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J40" s="4">
+        <f t="shared" si="0"/>
+        <v>41696.160000000003</v>
+      </c>
+      <c r="K40" s="4">
+        <f t="shared" si="1"/>
+        <v>2360.16</v>
+      </c>
+      <c r="L40" s="4">
+        <v>39336</v>
+      </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E41" s="2"/>
+      <c r="J41" s="4"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E42" s="2"/>

</xml_diff>